<commit_message>
update plots and saved 2d analytic parameters
</commit_message>
<xml_diff>
--- a/Trabajo_3/2D2R/Fit_model_2D2R.xlsx
+++ b/Trabajo_3/2D2R/Fit_model_2D2R.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Andres\1_Universidad\MUSE\GGE\Trabajos_GGE\Trabajo_3\2R2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Andres\1_Universidad\MUSE\GGE\Trabajos_GGE\Trabajo_3\2D2R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A361D2A-068B-48F2-B8E6-F38D9B6DB779}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8B5AA8-1F71-4F0C-9F23-7D1A0FF97652}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1944" yWindow="768" windowWidth="16404" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1944" yWindow="768" windowWidth="16404" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analitico" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>RTC France</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>4S1P</t>
+  </si>
+  <si>
+    <t>RMSE</t>
   </si>
 </sst>
 </file>
@@ -444,15 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06072C46-0D27-40DF-92FE-095DFA7E2FDC}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -477,112 +480,127 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.76200000000000001</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="C2">
-        <v>2.5600000000000002E-7</v>
+        <v>2.48E-6</v>
       </c>
       <c r="D2">
-        <v>2.6399999999999998E-7</v>
+        <v>-6.81E-6</v>
       </c>
       <c r="E2">
-        <v>3.7100000000000001E-2</v>
+        <v>3.5400000000000001E-2</v>
       </c>
       <c r="F2">
-        <v>44.6</v>
+        <v>45.2</v>
       </c>
       <c r="G2">
-        <v>1.46</v>
+        <v>1.67</v>
       </c>
       <c r="H2">
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.52600000000000002</v>
+        <v>0.52400000000000002</v>
       </c>
       <c r="C3" s="1">
-        <v>5.5700000000000002E-15</v>
+        <v>2.1999999999999999E-12</v>
       </c>
       <c r="D3" s="1">
-        <v>2.7000000000000001E-15</v>
+        <v>-3.3700000000000001E-9</v>
       </c>
       <c r="E3">
-        <v>0.105</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="F3">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G3">
-        <v>1.03</v>
+        <v>1.25</v>
       </c>
       <c r="H3">
-        <v>1.1299999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>7.26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.46400000000000002</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="C4" s="1">
-        <v>5.1099999999999998E-14</v>
+        <v>1.4700000000000002E-11</v>
       </c>
       <c r="D4" s="1">
-        <v>-6.9599999999999996E-13</v>
+        <v>-2.1200000000000001E-9</v>
       </c>
       <c r="E4">
-        <v>6.0900000000000003E-2</v>
+        <v>2.3400000000000001E-2</v>
       </c>
       <c r="F4">
-        <v>451</v>
+        <v>344</v>
       </c>
       <c r="G4">
-        <v>1.17</v>
+        <v>1.44</v>
       </c>
       <c r="H4">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.52700000000000002</v>
+        <v>0.52</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0599999999999999E-18</v>
+        <v>3.0400000000000002E-14</v>
       </c>
       <c r="D5" s="1">
-        <v>3.0699999999999998E-18</v>
+        <v>-1.38E-9</v>
       </c>
       <c r="E5">
-        <v>8.48E-2</v>
+        <v>9.7099999999999999E-3</v>
       </c>
       <c r="F5">
-        <v>3310</v>
+        <v>4780</v>
       </c>
       <c r="G5">
-        <v>0.85399999999999998</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H5">
-        <v>2.86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -590,155 +608,173 @@
         <v>1.03</v>
       </c>
       <c r="C6">
-        <v>1.72E-6</v>
+        <v>4.0800000000000002E-5</v>
       </c>
       <c r="D6">
-        <v>1.11E-6</v>
+        <v>-1.7000000000000001E-4</v>
       </c>
       <c r="E6">
-        <v>1.31</v>
+        <v>1.5</v>
       </c>
       <c r="F6">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="G6">
-        <v>1.28</v>
+        <v>1.58</v>
       </c>
       <c r="H6">
-        <v>4.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>8.19</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="C7" s="1">
-        <v>1.13E-9</v>
+        <v>2.2800000000000001E-4</v>
       </c>
       <c r="D7" s="1">
-        <v>5.2600000000000004E-10</v>
+        <v>-3.6499999999999998E-4</v>
       </c>
       <c r="E7">
-        <v>0.23899999999999999</v>
+        <v>0.193</v>
       </c>
       <c r="F7">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7">
-        <v>1.05</v>
+        <v>1.9</v>
       </c>
       <c r="H7">
-        <v>2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.499</v>
+        <v>0.504</v>
       </c>
       <c r="C8" s="1">
-        <v>7.3600000000000003E-17</v>
+        <v>3.5700000000000001E-10</v>
       </c>
       <c r="D8" s="1">
-        <v>4.9200000000000001E-16</v>
+        <v>-1.26E-8</v>
       </c>
       <c r="E8">
-        <v>0.11799999999999999</v>
+        <v>0.109</v>
       </c>
       <c r="F8">
-        <v>1580</v>
+        <v>775</v>
       </c>
       <c r="G8">
-        <v>0.98299999999999998</v>
+        <v>1.63</v>
       </c>
       <c r="H8">
-        <v>1.71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>7.54</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="C9">
-        <v>7.3499999999999998E-5</v>
+        <v>4.2899999999999999E-5</v>
       </c>
       <c r="D9">
-        <v>9.0600000000000007E-5</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="E9">
-        <v>-2.3700000000000001E-3</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="F9">
-        <v>0.20599999999999999</v>
+        <v>0.188</v>
       </c>
       <c r="G9">
-        <v>0.94799999999999995</v>
+        <v>4.7199999999999999E-2</v>
       </c>
       <c r="H9">
-        <v>0.99299999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.8</v>
+      </c>
+      <c r="I9">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>0.47399999999999998</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="C10" s="1">
-        <v>2.5000000000000001E-14</v>
+        <v>1.48E-12</v>
       </c>
       <c r="D10" s="1">
-        <v>2.0399999999999999E-13</v>
+        <v>-4.6000000000000001E-10</v>
       </c>
       <c r="E10">
-        <v>7.6300000000000007E-2</v>
+        <v>6.6600000000000006E-2</v>
       </c>
       <c r="F10">
-        <v>1340</v>
+        <v>66800</v>
       </c>
       <c r="G10">
-        <v>1.1100000000000001</v>
+        <v>1.28</v>
       </c>
       <c r="H10">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11">
-        <v>0.434</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>2.3799999999999999E-20</v>
+        <v>9.1900000000000002E-13</v>
       </c>
       <c r="D11" s="1">
-        <v>-4.8199999999999999E-20</v>
+        <v>-3.4200000000000002E-9</v>
       </c>
       <c r="E11">
-        <v>0.18</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="F11">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="G11">
-        <v>0.752</v>
+        <v>1.23</v>
       </c>
       <c r="H11">
-        <v>5.51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -746,22 +782,25 @@
         <v>0.46700000000000003</v>
       </c>
       <c r="C12" s="1">
-        <v>9.7200000000000002E-39</v>
+        <v>-2.4600000000000001E-43</v>
       </c>
       <c r="D12" s="1">
-        <v>6.6499999999999998E-37</v>
+        <v>7.3199999999999994E-38</v>
       </c>
       <c r="E12">
-        <v>1.27</v>
+        <v>0.89900000000000002</v>
       </c>
       <c r="F12">
-        <v>17800</v>
+        <v>6290</v>
       </c>
       <c r="G12">
+        <v>1.08</v>
+      </c>
+      <c r="H12">
         <v>1.24</v>
       </c>
-      <c r="H12">
-        <v>1.76</v>
+      <c r="I12">
+        <v>1.22</v>
       </c>
     </row>
   </sheetData>
@@ -771,15 +810,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D4C26D-EA37-4C87-A1F7-72F84F55EFAE}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -804,8 +843,11 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -830,8 +872,11 @@
       <c r="H2">
         <v>2.16</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -856,8 +901,11 @@
       <c r="H3">
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -882,8 +930,11 @@
       <c r="H4">
         <v>157</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -908,8 +959,11 @@
       <c r="H5">
         <v>2.86</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -934,8 +988,11 @@
       <c r="H6">
         <v>4.01</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -960,8 +1017,11 @@
       <c r="H7">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -986,8 +1046,11 @@
       <c r="H8">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1013,7 +1076,7 @@
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1102,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1065,7 +1128,7 @@
         <v>5.51</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>

</xml_diff>